<commit_message>
feat: update clase 7
</commit_message>
<xml_diff>
--- a/clase_7/resumen_ventas.xlsx
+++ b/clase_7/resumen_ventas.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,6 +477,7 @@
           <t>Productos_Vendidos</t>
         </is>
       </c>
+      <c r="H1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr"/>
@@ -510,6 +511,11 @@
           <t>mean</t>
         </is>
       </c>
+      <c r="H2" s="1" t="inlineStr">
+        <is>
+          <t>sum</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -542,6 +548,9 @@
       <c r="G4" t="n">
         <v>130</v>
       </c>
+      <c r="H4" t="n">
+        <v>520</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -567,9 +576,13 @@
       <c r="G5" t="n">
         <v>137.6666666666667</v>
       </c>
+      <c r="H5" t="n">
+        <v>413</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="G1:H1"/>
     <mergeCell ref="B1:F1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>